<commit_message>
all test suite excel updated
</commit_message>
<xml_diff>
--- a/bin/com/packagename/xls/Suite.xlsx
+++ b/bin/com/packagename/xls/Suite.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Automation-Test\NewWorkspace_2\HybridFramework_1\src\com\packagename\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Automation-Test\NewWorkspace_2\HybridFramework_1\bin\com\packagename\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Runmode</t>
   </si>
@@ -35,64 +35,94 @@
     <t>Navigate_Verification</t>
   </si>
   <si>
-    <t>Simple_Search</t>
-  </si>
-  <si>
-    <t>Create_Update_Classes</t>
-  </si>
-  <si>
-    <t>Create_Update_MonthlyGoal</t>
-  </si>
-  <si>
-    <t>Advance_Search_Verification</t>
-  </si>
-  <si>
-    <t>Delete_Verification</t>
-  </si>
-  <si>
-    <t>Assign_Verification</t>
-  </si>
-  <si>
-    <t>Logs_Verification</t>
-  </si>
-  <si>
-    <t>AccessModule_Verification</t>
-  </si>
-  <si>
-    <t>Assign_Student_Colors_Verification</t>
-  </si>
-  <si>
-    <t>Create_Update_Allsections</t>
-  </si>
-  <si>
-    <t>Special_Teachers</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Admin - Login Verification and Identify access type </t>
-  </si>
-  <si>
-    <t>Admin - Navigate All page - Content Verification</t>
-  </si>
-  <si>
-    <t>Simple Search Verification in all sections</t>
-  </si>
-  <si>
-    <t>Crud Opteration verification in all section</t>
-  </si>
-  <si>
-    <t>Crud Opteration verification in class sections</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
     <t>TSID</t>
+  </si>
+  <si>
+    <t>Product_Verification</t>
+  </si>
+  <si>
+    <t>AddToCart_Verification</t>
+  </si>
+  <si>
+    <t>Order_Module</t>
+  </si>
+  <si>
+    <t>EvolveMoney_Module</t>
+  </si>
+  <si>
+    <t>GiftVoucher_Module</t>
+  </si>
+  <si>
+    <t>Hamper_Module</t>
+  </si>
+  <si>
+    <t>Browser_Verification</t>
+  </si>
+  <si>
+    <t>Registeration_Verification</t>
+  </si>
+  <si>
+    <t>Subscription_Module</t>
+  </si>
+  <si>
+    <t>Form_Verification</t>
+  </si>
+  <si>
+    <t>Link_Verification</t>
+  </si>
+  <si>
+    <t>Gift Voucher based Test Cases</t>
+  </si>
+  <si>
+    <t>All type of login execute</t>
+  </si>
+  <si>
+    <t>Navigation based Test Cases execute</t>
+  </si>
+  <si>
+    <t>All Products based Test Cases execute</t>
+  </si>
+  <si>
+    <t>Add all type of product based Test Cases execute</t>
+  </si>
+  <si>
+    <t>Order status  based Test Cases execute</t>
+  </si>
+  <si>
+    <t>Evolve money based Test Cases execute</t>
+  </si>
+  <si>
+    <t>Referal based Test Cases execute</t>
+  </si>
+  <si>
+    <t>Referral _Module</t>
+  </si>
+  <si>
+    <t>Hamper_Module based Test Cases</t>
+  </si>
+  <si>
+    <t>Subscription_Module based Test Cases</t>
+  </si>
+  <si>
+    <t>Form_Verification based Test Cases</t>
+  </si>
+  <si>
+    <t>Link_Verification based Test Cases</t>
+  </si>
+  <si>
+    <t>Browser_Verification based Test Cases</t>
+  </si>
+  <si>
+    <t>Registeration_Verification based Test Cases</t>
   </si>
 </sst>
 </file>
@@ -432,25 +462,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="1" max="1" width="37.5703125" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -461,10 +491,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -472,131 +502,142 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>